<commit_message>
Download and unarchive scanned pdfs.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diana.prisecaru\Projects\R&amp;D\Accesa.RPA.SnippetsAndTemplates\Framework_Performer_NoQueue\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giorgia.cocis\Desktop\SDD and Estimations\VoteCounter\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E684FF2-77E1-4E4C-9929-86890758C19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A33BC2-0610-4B77-A0BA-1DF2A977C583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>Name</t>
   </si>
@@ -402,6 +402,42 @@
   </si>
   <si>
     <t>Static part of logging message. Robot failed with initialization exception.</t>
+  </si>
+  <si>
+    <t>C:\Users\giorgia.cocis\Desktop\SDD and Estimations</t>
+  </si>
+  <si>
+    <t>Path_DownloadFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\giorgia.cocis\Desktop\SDD and Estimations\VoteCounter\Data\Input</t>
+  </si>
+  <si>
+    <t>Path_InputFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\giorgia.cocis\Desktop\SDD and Estimations\ScannedVotes.zip</t>
+  </si>
+  <si>
+    <t>Path_SourceFolder</t>
+  </si>
+  <si>
+    <t>The path of the folder where the archive is being downloaded.</t>
+  </si>
+  <si>
+    <t>The path of the folder where the files are being unarchived.</t>
+  </si>
+  <si>
+    <t>The path of the folder containing the archive.</t>
+  </si>
+  <si>
+    <t>Path_VotesFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\giorgia.cocis\Desktop\SDD and Estimations\VoteCounter\Data\Input\ScannedVotes</t>
+  </si>
+  <si>
+    <t>The path of the folder containing the scanned pdfs.</t>
   </si>
 </sst>
 </file>
@@ -836,18 +872,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1012"/>
+  <dimension ref="A1:Z1015"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="105.44140625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="87.33203125" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="105.453125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="87.36328125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1006,7 +1042,7 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:26" ht="28.8">
+    <row r="6" spans="1:26" ht="29">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -1017,11 +1053,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.4">
+    <row r="7" spans="1:26" ht="14.5">
       <c r="B7" s="18"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:26" s="10" customFormat="1" ht="14.4">
+    <row r="8" spans="1:26" s="10" customFormat="1" ht="14.5">
       <c r="A8" s="9" t="s">
         <v>47</v>
       </c>
@@ -1039,177 +1075,217 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" s="10" customFormat="1" ht="14.4">
-      <c r="A11" s="9" t="s">
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" s="10" customFormat="1" ht="14.5">
+      <c r="A14" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:26" s="12" customFormat="1" ht="14.4">
-      <c r="A12" s="25"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="13"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" s="10" customFormat="1" ht="14.4">
-      <c r="A14" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="B14" s="19"/>
       <c r="C14" s="11"/>
     </row>
-    <row r="15" spans="1:26" s="12" customFormat="1" ht="14.4">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:26" s="12" customFormat="1" ht="14.5">
+      <c r="A15" s="25"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="13"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" s="10" customFormat="1" ht="14.5">
+      <c r="A17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="11"/>
+    </row>
+    <row r="18" spans="1:3" s="12" customFormat="1" ht="14.5">
+      <c r="A18" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="21" t="b">
+      <c r="B18" s="21" t="b">
         <v>1</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C18" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:26" s="12" customFormat="1" ht="14.4">
-      <c r="A16" s="14"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:3" s="12" customFormat="1" ht="14.4">
-      <c r="A17" s="14" t="s">
+    <row r="19" spans="1:3" s="12" customFormat="1" ht="14.5">
+      <c r="A19" s="14"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:3" s="12" customFormat="1" ht="14.5">
+      <c r="A20" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B20" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="13"/>
-    </row>
-    <row r="18" spans="1:3" s="12" customFormat="1" ht="14.4">
-      <c r="A18" s="14"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" s="12" customFormat="1" ht="86.4">
-      <c r="A19" s="14" t="s">
+      <c r="C20" s="13"/>
+    </row>
+    <row r="21" spans="1:3" s="12" customFormat="1" ht="14.5">
+      <c r="A21" s="14"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:3" s="12" customFormat="1" ht="87">
+      <c r="A22" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B22" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="13"/>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
+      <c r="C22" s="13"/>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B24" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B25" s="18" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="201.6">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.4">
-      <c r="B25" s="24"/>
-      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="203">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.5">
+      <c r="B28" s="24"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B29" s="18" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A27" t="s">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B30" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" t="s">
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="201.6">
-      <c r="A29" t="s">
+    <row r="32" spans="1:3" ht="203">
+      <c r="A32" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B32" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.4">
-      <c r="A31" t="s">
+    <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:2" ht="14.5">
+      <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B34" s="18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" t="s">
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B35" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="158.4">
-      <c r="A34" s="3" t="s">
+    <row r="37" spans="1:2" ht="159.5">
+      <c r="A37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="24" t="s">
+      <c r="B37" s="24" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B42"/>
-    </row>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1">
+      <c r="B45"/>
+    </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2177,6 +2253,9 @@
     <row r="1010" ht="14.25" customHeight="1"/>
     <row r="1011" ht="14.25" customHeight="1"/>
     <row r="1012" ht="14.25" customHeight="1"/>
+    <row r="1013" ht="14.25" customHeight="1"/>
+    <row r="1014" ht="14.25" customHeight="1"/>
+    <row r="1015" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2188,16 +2267,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.6328125" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2234,7 +2313,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2245,7 +2324,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.8">
+    <row r="3" spans="1:26" ht="29">
       <c r="A3" s="3" t="s">
         <v>94</v>
       </c>
@@ -3457,12 +3536,12 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.90625" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="60.36328125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3531,7 +3610,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="12" customFormat="1" ht="14.4">
+    <row r="9" spans="1:26" s="12" customFormat="1" ht="14.5">
       <c r="C9" s="13"/>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>